<commit_message>
added a spreadsheet to visualize the db better
</commit_message>
<xml_diff>
--- a/Gas Inventory Spreadsheet.xlsx
+++ b/Gas Inventory Spreadsheet.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gas-inventory-management-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9151CC70-5887-4CA3-8EA0-5E2686CB1023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAD9640-CBE9-4225-8C81-A21BCDA93A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
     <sheet name="Shift" sheetId="2" r:id="rId2"/>
-    <sheet name="Transaction" sheetId="3" r:id="rId3"/>
-    <sheet name="Tank Fuel Inventory" sheetId="4" r:id="rId4"/>
-    <sheet name="Fuel Types" sheetId="5" r:id="rId5"/>
-    <sheet name="Deliveries" sheetId="6" r:id="rId6"/>
-    <sheet name="Price" sheetId="7" r:id="rId7"/>
-    <sheet name="Fuel Pump" sheetId="8" r:id="rId8"/>
+    <sheet name="Fuel Pump" sheetId="8" r:id="rId3"/>
+    <sheet name="Price" sheetId="7" r:id="rId4"/>
+    <sheet name="Transaction" sheetId="3" r:id="rId5"/>
+    <sheet name="Fuel Tank Inventory" sheetId="4" r:id="rId6"/>
+    <sheet name="Fuel_type" sheetId="9" r:id="rId7"/>
+    <sheet name="Deliveries" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,15 +43,126 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>Password_hash</t>
+  </si>
+  <si>
+    <t>Shift Id</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>User_id</t>
+  </si>
+  <si>
+    <t>Transaction_id</t>
+  </si>
+  <si>
+    <t>Shift_Date</t>
+  </si>
+  <si>
+    <t>Shift_type</t>
+  </si>
+  <si>
+    <t>Start_time</t>
+  </si>
+  <si>
+    <t>End_time</t>
+  </si>
+  <si>
+    <t>Pump_id</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Transaction_Datetime</t>
+  </si>
+  <si>
+    <t>Price_id</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Effective_date</t>
+  </si>
+  <si>
+    <t>Fuel_type_id</t>
+  </si>
+  <si>
+    <t>Pump_label</t>
+  </si>
+  <si>
+    <t>Fuel_name</t>
+  </si>
+  <si>
+    <t>Unleaded</t>
+  </si>
+  <si>
+    <t>Premium 3</t>
+  </si>
+  <si>
+    <t>Premium 2</t>
+  </si>
+  <si>
+    <t>Premium 1</t>
+  </si>
+  <si>
+    <t>Diesel 1</t>
+  </si>
+  <si>
+    <t>Diesel 2</t>
+  </si>
+  <si>
+    <t>Fuel_Tank_id</t>
+  </si>
+  <si>
+    <t>Shift_id</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
+    <t>shift_id</t>
+  </si>
+  <si>
+    <t>Volume_delivered</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>sdadsada</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>END_Volume_Dispensed</t>
+  </si>
+  <si>
+    <t>datetime</t>
   </si>
 </sst>
 </file>
@@ -423,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7D3F36-7ED1-4DEE-8CEF-A514911495B0}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,13 +548,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -453,53 +583,613 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41CCF1E-B44C-4D23-B730-915B6A2ABEA6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C125461B-8C6E-43D6-B35D-90809A380C95}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9AA574-A4A8-4D18-B70B-DF537F0C161E}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5508EC-71B8-4159-857F-F3C483193968}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FFFE0D-90A2-4AC9-A995-57C5BBB3651F}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C821A3-0198-477F-834A-7E62895D8E46}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C125461B-8C6E-43D6-B35D-90809A380C95}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>400</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5508EC-71B8-4159-857F-F3C483193968}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AA0522-5B61-4156-A69F-5D553B21F107}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F265EA81-064F-4D5F-B839-B754DA93C013}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -509,28 +1199,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FFFE0D-90A2-4AC9-A995-57C5BBB3651F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9AA574-A4A8-4D18-B70B-DF537F0C161E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added values for visualization
</commit_message>
<xml_diff>
--- a/Gas Inventory Spreadsheet.xlsx
+++ b/Gas Inventory Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gas-inventory-management-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAD9640-CBE9-4225-8C81-A21BCDA93A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CBB06B-03EA-410C-B7EE-0BD63F5F11C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>username</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>datetime</t>
+  </si>
+  <si>
+    <t>fwefgwwgrw</t>
   </si>
 </sst>
 </file>
@@ -575,6 +578,9 @@
       <c r="B3" t="s">
         <v>33</v>
       </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -690,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9AA574-A4A8-4D18-B70B-DF537F0C161E}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -788,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FFFE0D-90A2-4AC9-A995-57C5BBB3651F}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,7 +1064,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,10 +1143,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AA0522-5B61-4156-A69F-5D553B21F107}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,18 +1155,15 @@
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
improved visualization of the databases by adding values to the table
</commit_message>
<xml_diff>
--- a/Gas Inventory Spreadsheet.xlsx
+++ b/Gas Inventory Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gas-inventory-management-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CBB06B-03EA-410C-B7EE-0BD63F5F11C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A7D62E-7E94-46E0-A201-0BD83931DD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41CCF1E-B44C-4D23-B730-915B6A2ABEA6}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9AA574-A4A8-4D18-B70B-DF537F0C161E}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added pump and fuel_type tables and fixed bugs
</commit_message>
<xml_diff>
--- a/Gas Inventory Spreadsheet.xlsx
+++ b/Gas Inventory Spreadsheet.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gas-inventory-management-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BF7D5D-E45B-4F52-ACB9-8F12368DDB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C656F112-FE2A-43DF-845D-792392443377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
     <sheet name="Shift" sheetId="2" r:id="rId2"/>
-    <sheet name="Fuel Pump" sheetId="8" r:id="rId3"/>
-    <sheet name="Price" sheetId="7" r:id="rId4"/>
-    <sheet name="Transaction" sheetId="3" r:id="rId5"/>
-    <sheet name="Fuel Tank Inventory" sheetId="4" r:id="rId6"/>
-    <sheet name="Fuel_type" sheetId="9" r:id="rId7"/>
+    <sheet name="Fuel_type" sheetId="9" r:id="rId3"/>
+    <sheet name="Fuel Pump" sheetId="8" r:id="rId4"/>
+    <sheet name="Price" sheetId="7" r:id="rId5"/>
+    <sheet name="Transaction" sheetId="3" r:id="rId6"/>
+    <sheet name="Fuel Tank Inventory" sheetId="4" r:id="rId7"/>
     <sheet name="Deliveries" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
@@ -117,9 +117,6 @@
     <t>shift_id</t>
   </si>
   <si>
-    <t>Volume_delivered</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -160,6 +157,12 @@
   </si>
   <si>
     <t>shift_date</t>
+  </si>
+  <si>
+    <t>Delivery_id</t>
+  </si>
+  <si>
+    <t>Supplier</t>
   </si>
 </sst>
 </file>
@@ -559,10 +562,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -570,10 +573,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41CCF1E-B44C-4D23-B730-915B6A2ABEA6}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -609,16 +612,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -629,16 +632,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -649,16 +652,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -669,16 +672,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -687,11 +690,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AA0522-5B61-4156-A69F-5D553B21F107}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9AA574-A4A8-4D18-B70B-DF537F0C161E}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FFFE0D-90A2-4AC9-A995-57C5BBB3651F}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -824,7 +879,7 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -838,7 +893,7 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -852,7 +907,7 @@
         <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -866,7 +921,7 @@
         <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -880,7 +935,7 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -894,7 +949,7 @@
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -908,7 +963,7 @@
         <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -922,7 +977,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -930,7 +985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C125461B-8C6E-43D6-B35D-90809A380C95}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -977,7 +1032,7 @@
         <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -994,7 +1049,7 @@
         <v>3000</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1011,7 +1066,7 @@
         <v>3000</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1028,7 +1083,7 @@
         <v>400</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1045,7 +1100,7 @@
         <v>300</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1053,12 +1108,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5508EC-71B8-4159-857F-F3C483193968}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,7 +1126,7 @@
     <col min="6" max="6" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1082,13 +1137,10 @@
         <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1102,7 +1154,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1116,7 +1168,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1128,57 +1180,6 @@
       </c>
       <c r="D4">
         <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AA0522-5B61-4156-A69F-5D553B21F107}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1188,12 +1189,34 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F265EA81-064F-4D5F-B839-B754DA93C013}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added a functioning updatable price table
</commit_message>
<xml_diff>
--- a/Gas Inventory Spreadsheet.xlsx
+++ b/Gas Inventory Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gas-inventory-management-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C656F112-FE2A-43DF-845D-792392443377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DAED21-39D4-4804-821C-D5921A837A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CA9EBFFD-BFCC-4E7A-B144-037E8AA9DE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>username</t>
   </si>
@@ -163,6 +163,21 @@
   </si>
   <si>
     <t>Supplier</t>
+  </si>
+  <si>
+    <t>fuel_type_id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Diesel100</t>
+  </si>
+  <si>
+    <t>Premium100</t>
+  </si>
+  <si>
+    <t>Unleaded100</t>
   </si>
 </sst>
 </file>
@@ -745,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9AA574-A4A8-4D18-B70B-DF537F0C161E}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -841,10 +856,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FFFE0D-90A2-4AC9-A995-57C5BBB3651F}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,131 +867,159 @@
     <col min="2" max="2" width="12.109375" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
         <v>70</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5">
         <v>60</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6">
         <v>60</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8">
         <v>60</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
         <v>60</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>